<commit_message>
changed base tag color to special clearance yellow for now
</commit_message>
<xml_diff>
--- a/democust.xlsx
+++ b/democust.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">SKU</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Parts Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">HP 933 XL Ink</t>
@@ -161,7 +164,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -217,14 +220,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>6802301</v>
+      <c r="A2" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>999.99</v>
@@ -242,7 +245,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>1</v>

</xml_diff>